<commit_message>
Add manual validation script for postprocessing.
</commit_message>
<xml_diff>
--- a/processed_data/small_validation_data/kmeans_results.xlsx
+++ b/processed_data/small_validation_data/kmeans_results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="265">
   <si>
     <t>fname</t>
   </si>
@@ -655,6 +655,81 @@
   </si>
   <si>
     <t>dp_pcm</t>
+  </si>
+  <si>
+    <t>dp</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0024.tif</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0025.tif</t>
+  </si>
+  <si>
+    <t>c3_344b_2203K_4.9atm_0008.tif</t>
+  </si>
+  <si>
+    <t>c3_344b_2203K_4.9atm_0012.tif</t>
+  </si>
+  <si>
+    <t>c3_344b_2203K_4.9atm_0013.tif</t>
+  </si>
+  <si>
+    <t>c3_344b_2203K_4.9atm_0014.tif</t>
+  </si>
+  <si>
+    <t>c3_344b_2203K_4.9atm_0015.tif</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>img_id</t>
+  </si>
+  <si>
+    <t>pixsize</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>aspect_ratio</t>
+  </si>
+  <si>
+    <t>num_pixels</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>Rg</t>
+  </si>
+  <si>
+    <t>perimeter</t>
+  </si>
+  <si>
+    <t>circularity</t>
+  </si>
+  <si>
+    <t>zbar_opt</t>
+  </si>
+  <si>
+    <t>center_mass_1</t>
+  </si>
+  <si>
+    <t>center_mass_2</t>
+  </si>
+  <si>
+    <t>dp_kook</t>
   </si>
   <si>
     <t>dp</t>
@@ -753,7 +828,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -770,11 +845,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -785,6 +861,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -819,63 +896,63 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>223</v>
+        <v>248</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>224</v>
+        <v>249</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>225</v>
+        <v>250</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>226</v>
+        <v>251</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>227</v>
+        <v>252</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>228</v>
+        <v>253</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>229</v>
+        <v>254</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>230</v>
+        <v>255</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>231</v>
+        <v>256</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>232</v>
+        <v>257</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>233</v>
+        <v>258</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>234</v>
+        <v>259</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>235</v>
+        <v>260</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>236</v>
+        <v>261</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>237</v>
+        <v>262</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>238</v>
+        <v>263</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>239</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="B2" s="0">
         <v>1</v>
@@ -931,7 +1008,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="B3" s="0">
         <v>2</v>
@@ -987,7 +1064,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="B4" s="0">
         <v>3</v>
@@ -1039,7 +1116,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="B5" s="0">
         <v>4</v>
@@ -1095,7 +1172,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="B6" s="0">
         <v>5</v>
@@ -1151,7 +1228,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
       <c r="B7" s="0">
         <v>6</v>
@@ -1207,7 +1284,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
       <c r="B8" s="0">
         <v>7</v>
@@ -1263,7 +1340,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
       <c r="B9" s="0">
         <v>8</v>
@@ -1319,7 +1396,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
       <c r="B10" s="0">
         <v>9</v>
@@ -1375,7 +1452,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
       <c r="B11" s="0">
         <v>10</v>
@@ -1431,7 +1508,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
       <c r="B12" s="0">
         <v>11</v>
@@ -1487,7 +1564,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="B13" s="0">
         <v>12</v>
@@ -1543,7 +1620,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="B14" s="0">
         <v>13</v>
@@ -1599,7 +1676,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="B15" s="0">
         <v>14</v>
@@ -1655,7 +1732,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="B16" s="0">
         <v>15</v>
@@ -1711,7 +1788,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="B17" s="0">
         <v>16</v>
@@ -1763,7 +1840,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="B18" s="0">
         <v>17</v>
@@ -1819,7 +1896,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="B19" s="0">
         <v>18</v>
@@ -1871,7 +1948,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="B20" s="0">
         <v>19</v>
@@ -1923,7 +2000,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>219</v>
+        <v>244</v>
       </c>
       <c r="B21" s="0">
         <v>20</v>
@@ -1979,7 +2056,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>219</v>
+        <v>244</v>
       </c>
       <c r="B22" s="0">
         <v>21</v>
@@ -2035,7 +2112,7 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>219</v>
+        <v>244</v>
       </c>
       <c r="B23" s="0">
         <v>22</v>
@@ -2087,7 +2164,7 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="B24" s="0">
         <v>23</v>
@@ -2139,7 +2216,7 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="B25" s="0">
         <v>24</v>
@@ -2195,7 +2272,7 @@
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="B26" s="0">
         <v>25</v>
@@ -2251,7 +2328,7 @@
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="B27" s="0">
         <v>26</v>
@@ -2303,7 +2380,7 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="B28" s="0">
         <v>27</v>
@@ -2359,7 +2436,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="B29" s="0">
         <v>28</v>
@@ -2415,7 +2492,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="B30" s="0">
         <v>29</v>
@@ -2471,7 +2548,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="B31" s="0">
         <v>30</v>
@@ -2523,7 +2600,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="B32" s="0">
         <v>31</v>
@@ -2575,7 +2652,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="B33" s="0">
         <v>32</v>
@@ -2631,7 +2708,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="B34" s="0">
         <v>33</v>
@@ -2687,7 +2764,7 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="B35" s="0">
         <v>34</v>
@@ -2739,7 +2816,7 @@
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="B36" s="0">
         <v>35</v>
@@ -2791,7 +2868,7 @@
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="B37" s="0">
         <v>36</v>
@@ -2847,7 +2924,7 @@
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="B38" s="0">
         <v>37</v>
@@ -2903,7 +2980,7 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="B39" s="0">
         <v>38</v>
@@ -2959,7 +3036,7 @@
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="B40" s="0">
         <v>39</v>
@@ -3015,7 +3092,7 @@
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="B41" s="0">
         <v>40</v>
@@ -3071,7 +3148,7 @@
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="B42" s="0">
         <v>41</v>
@@ -3127,7 +3204,7 @@
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="B43" s="0">
         <v>42</v>
@@ -3183,7 +3260,7 @@
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="B44" s="0">
         <v>43</v>
@@ -3235,7 +3312,7 @@
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="B45" s="0">
         <v>44</v>
@@ -3287,7 +3364,7 @@
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="B46" s="0">
         <v>45</v>
@@ -3339,7 +3416,7 @@
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="B47" s="0">
         <v>46</v>
@@ -3391,7 +3468,7 @@
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="B48" s="0">
         <v>47</v>
@@ -3443,7 +3520,7 @@
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="B49" s="0">
         <v>48</v>
@@ -3499,7 +3576,7 @@
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="B50" s="0">
         <v>49</v>
@@ -3551,7 +3628,7 @@
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="B51" s="0">
         <v>50</v>
@@ -3603,7 +3680,7 @@
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="B52" s="0">
         <v>51</v>
@@ -3659,7 +3736,7 @@
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="B53" s="0">
         <v>52</v>
@@ -3715,7 +3792,7 @@
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="B54" s="0">
         <v>53</v>
@@ -3771,7 +3848,7 @@
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="B55" s="0">
         <v>54</v>
@@ -3823,7 +3900,7 @@
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="B56" s="0">
         <v>55</v>
@@ -3875,7 +3952,7 @@
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="B57" s="0">
         <v>56</v>
@@ -3931,7 +4008,7 @@
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="B58" s="0">
         <v>57</v>
@@ -3987,7 +4064,7 @@
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="B59" s="0">
         <v>58</v>
@@ -4043,7 +4120,7 @@
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="B60" s="0">
         <v>59</v>
@@ -4095,7 +4172,7 @@
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="B61" s="0">
         <v>60</v>

</xml_diff>

<commit_message>
Histograms now filter for image zoom level and manual exclusions. Much improved!
</commit_message>
<xml_diff>
--- a/processed_data/small_validation_data/kmeans_results.xlsx
+++ b/processed_data/small_validation_data/kmeans_results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="290">
   <si>
     <t>fname</t>
   </si>
@@ -655,6 +655,81 @@
   </si>
   <si>
     <t>dp_pcm</t>
+  </si>
+  <si>
+    <t>dp</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0024.tif</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0025.tif</t>
+  </si>
+  <si>
+    <t>c3_344b_2203K_4.9atm_0008.tif</t>
+  </si>
+  <si>
+    <t>c3_344b_2203K_4.9atm_0012.tif</t>
+  </si>
+  <si>
+    <t>c3_344b_2203K_4.9atm_0013.tif</t>
+  </si>
+  <si>
+    <t>c3_344b_2203K_4.9atm_0014.tif</t>
+  </si>
+  <si>
+    <t>c3_344b_2203K_4.9atm_0015.tif</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>img_id</t>
+  </si>
+  <si>
+    <t>pixsize</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>aspect_ratio</t>
+  </si>
+  <si>
+    <t>num_pixels</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>Rg</t>
+  </si>
+  <si>
+    <t>perimeter</t>
+  </si>
+  <si>
+    <t>circularity</t>
+  </si>
+  <si>
+    <t>zbar_opt</t>
+  </si>
+  <si>
+    <t>center_mass_1</t>
+  </si>
+  <si>
+    <t>center_mass_2</t>
+  </si>
+  <si>
+    <t>dp_kook</t>
   </si>
   <si>
     <t>dp</t>
@@ -828,7 +903,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -846,11 +921,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -862,6 +938,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -896,63 +973,63 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>248</v>
+        <v>273</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>251</v>
+        <v>276</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>252</v>
+        <v>277</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>253</v>
+        <v>278</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>254</v>
+        <v>279</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>255</v>
+        <v>280</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>257</v>
+        <v>282</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>258</v>
+        <v>283</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>259</v>
+        <v>284</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>260</v>
+        <v>285</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>261</v>
+        <v>286</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>262</v>
+        <v>287</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>263</v>
+        <v>288</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>264</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="B2" s="0">
         <v>1</v>
@@ -1008,7 +1085,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="B3" s="0">
         <v>2</v>
@@ -1064,7 +1141,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="B4" s="0">
         <v>3</v>
@@ -1116,7 +1193,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="B5" s="0">
         <v>4</v>
@@ -1172,7 +1249,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="B6" s="0">
         <v>5</v>
@@ -1228,7 +1305,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>242</v>
+        <v>267</v>
       </c>
       <c r="B7" s="0">
         <v>6</v>
@@ -1284,7 +1361,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>242</v>
+        <v>267</v>
       </c>
       <c r="B8" s="0">
         <v>7</v>
@@ -1340,7 +1417,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>242</v>
+        <v>267</v>
       </c>
       <c r="B9" s="0">
         <v>8</v>
@@ -1396,7 +1473,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>242</v>
+        <v>267</v>
       </c>
       <c r="B10" s="0">
         <v>9</v>
@@ -1452,7 +1529,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>242</v>
+        <v>267</v>
       </c>
       <c r="B11" s="0">
         <v>10</v>
@@ -1508,7 +1585,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>242</v>
+        <v>267</v>
       </c>
       <c r="B12" s="0">
         <v>11</v>
@@ -1564,7 +1641,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
       <c r="B13" s="0">
         <v>12</v>
@@ -1620,7 +1697,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
       <c r="B14" s="0">
         <v>13</v>
@@ -1676,7 +1753,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
       <c r="B15" s="0">
         <v>14</v>
@@ -1732,7 +1809,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
       <c r="B16" s="0">
         <v>15</v>
@@ -1788,7 +1865,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
       <c r="B17" s="0">
         <v>16</v>
@@ -1840,7 +1917,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
       <c r="B18" s="0">
         <v>17</v>
@@ -1896,7 +1973,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
       <c r="B19" s="0">
         <v>18</v>
@@ -1948,7 +2025,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
       <c r="B20" s="0">
         <v>19</v>
@@ -2000,7 +2077,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>244</v>
+        <v>269</v>
       </c>
       <c r="B21" s="0">
         <v>20</v>
@@ -2056,7 +2133,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>244</v>
+        <v>269</v>
       </c>
       <c r="B22" s="0">
         <v>21</v>
@@ -2112,7 +2189,7 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>244</v>
+        <v>269</v>
       </c>
       <c r="B23" s="0">
         <v>22</v>
@@ -2164,7 +2241,7 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="B24" s="0">
         <v>23</v>
@@ -2216,7 +2293,7 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="B25" s="0">
         <v>24</v>
@@ -2272,7 +2349,7 @@
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="B26" s="0">
         <v>25</v>
@@ -2328,7 +2405,7 @@
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="B27" s="0">
         <v>26</v>
@@ -2380,7 +2457,7 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="B28" s="0">
         <v>27</v>
@@ -2436,7 +2513,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="B29" s="0">
         <v>28</v>
@@ -2492,7 +2569,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="B30" s="0">
         <v>29</v>
@@ -2548,7 +2625,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="B31" s="0">
         <v>30</v>
@@ -2600,7 +2677,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="B32" s="0">
         <v>31</v>
@@ -2652,7 +2729,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="B33" s="0">
         <v>32</v>
@@ -2708,7 +2785,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="B34" s="0">
         <v>33</v>
@@ -2764,7 +2841,7 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="B35" s="0">
         <v>34</v>
@@ -2816,7 +2893,7 @@
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="B36" s="0">
         <v>35</v>
@@ -2868,7 +2945,7 @@
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="B37" s="0">
         <v>36</v>
@@ -2924,7 +3001,7 @@
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="B38" s="0">
         <v>37</v>
@@ -2980,7 +3057,7 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="B39" s="0">
         <v>38</v>
@@ -3036,7 +3113,7 @@
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="B40" s="0">
         <v>39</v>
@@ -3092,7 +3169,7 @@
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="B41" s="0">
         <v>40</v>
@@ -3148,7 +3225,7 @@
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="B42" s="0">
         <v>41</v>
@@ -3204,7 +3281,7 @@
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="B43" s="0">
         <v>42</v>
@@ -3260,7 +3337,7 @@
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="B44" s="0">
         <v>43</v>
@@ -3312,7 +3389,7 @@
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="B45" s="0">
         <v>44</v>
@@ -3364,7 +3441,7 @@
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="B46" s="0">
         <v>45</v>
@@ -3416,7 +3493,7 @@
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B47" s="0">
         <v>46</v>
@@ -3468,7 +3545,7 @@
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B48" s="0">
         <v>47</v>
@@ -3520,7 +3597,7 @@
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B49" s="0">
         <v>48</v>
@@ -3576,7 +3653,7 @@
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B50" s="0">
         <v>49</v>
@@ -3628,7 +3705,7 @@
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B51" s="0">
         <v>50</v>
@@ -3680,7 +3757,7 @@
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B52" s="0">
         <v>51</v>
@@ -3736,7 +3813,7 @@
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B53" s="0">
         <v>52</v>
@@ -3792,7 +3869,7 @@
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B54" s="0">
         <v>53</v>
@@ -3848,7 +3925,7 @@
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B55" s="0">
         <v>54</v>
@@ -3900,7 +3977,7 @@
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B56" s="0">
         <v>55</v>
@@ -3952,7 +4029,7 @@
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B57" s="0">
         <v>56</v>
@@ -4008,7 +4085,7 @@
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B58" s="0">
         <v>57</v>
@@ -4064,7 +4141,7 @@
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B59" s="0">
         <v>58</v>
@@ -4120,7 +4197,7 @@
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B60" s="0">
         <v>59</v>
@@ -4172,7 +4249,7 @@
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B61" s="0">
         <v>60</v>

</xml_diff>